<commit_message>
added UPH to regular pick and changed to abs intead of negative in regular pick
</commit_message>
<xml_diff>
--- a/pick_counts.xlsx
+++ b/pick_counts.xlsx
@@ -576,7 +576,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -595,6 +595,11 @@
           <t>RegularPickQuantity</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>UPH</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -603,7 +608,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-20</v>
+        <v>20</v>
+      </c>
+      <c r="C2" t="n">
+        <v>7.100591715976331</v>
       </c>
     </row>
     <row r="3">
@@ -613,7 +621,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-52</v>
+        <v>52</v>
+      </c>
+      <c r="C3" t="n">
+        <v>18.46153846153846</v>
       </c>
     </row>
     <row r="4">
@@ -623,7 +634,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-1</v>
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.3550295857988165</v>
       </c>
     </row>
     <row r="5">
@@ -633,7 +647,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-33</v>
+        <v>33</v>
+      </c>
+      <c r="C5" t="n">
+        <v>11.71597633136095</v>
       </c>
     </row>
     <row r="6">
@@ -643,7 +660,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-6</v>
+        <v>6</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2.130177514792899</v>
       </c>
     </row>
     <row r="7">
@@ -653,7 +673,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-21</v>
+        <v>21</v>
+      </c>
+      <c r="C7" t="n">
+        <v>7.455621301775148</v>
       </c>
     </row>
     <row r="8">
@@ -663,7 +686,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-2</v>
+        <v>2</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.7100591715976331</v>
       </c>
     </row>
     <row r="9">
@@ -673,7 +699,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-12</v>
+        <v>12</v>
+      </c>
+      <c r="C9" t="n">
+        <v>4.260355029585798</v>
       </c>
     </row>
     <row r="10">
@@ -683,7 +712,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-11</v>
+        <v>11</v>
+      </c>
+      <c r="C10" t="n">
+        <v>3.905325443786982</v>
       </c>
     </row>
     <row r="11">
@@ -693,7 +725,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-25</v>
+        <v>25</v>
+      </c>
+      <c r="C11" t="n">
+        <v>8.875739644970414</v>
       </c>
     </row>
     <row r="12">
@@ -703,7 +738,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-15</v>
+        <v>15</v>
+      </c>
+      <c r="C12" t="n">
+        <v>5.325443786982248</v>
       </c>
     </row>
     <row r="13">
@@ -713,7 +751,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-31</v>
+        <v>31</v>
+      </c>
+      <c r="C13" t="n">
+        <v>11.00591715976331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added UPH to replenishment pick and changed it to positive numbers
</commit_message>
<xml_diff>
--- a/pick_counts.xlsx
+++ b/pick_counts.xlsx
@@ -889,7 +889,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -908,6 +908,11 @@
           <t>ReplenishmentPickQuantity</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>UPH</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -916,7 +921,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-64</v>
+        <v>64</v>
+      </c>
+      <c r="C2" t="n">
+        <v>25.26315789473684</v>
       </c>
     </row>
     <row r="3">
@@ -926,7 +934,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-60</v>
+        <v>60</v>
+      </c>
+      <c r="C3" t="n">
+        <v>23.68421052631579</v>
       </c>
     </row>
     <row r="4">
@@ -936,7 +947,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-89</v>
+        <v>89</v>
+      </c>
+      <c r="C4" t="n">
+        <v>35.13157894736842</v>
       </c>
     </row>
     <row r="5">
@@ -946,7 +960,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-90</v>
+        <v>90</v>
+      </c>
+      <c r="C5" t="n">
+        <v>35.52631578947368</v>
       </c>
     </row>
     <row r="6">
@@ -956,7 +973,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-48</v>
+        <v>48</v>
+      </c>
+      <c r="C6" t="n">
+        <v>18.94736842105263</v>
       </c>
     </row>
     <row r="7">
@@ -966,7 +986,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-38</v>
+        <v>38</v>
+      </c>
+      <c r="C7" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="8">
@@ -976,7 +999,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-76</v>
+        <v>76</v>
+      </c>
+      <c r="C8" t="n">
+        <v>30</v>
       </c>
     </row>
     <row r="9">
@@ -986,7 +1012,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-54</v>
+        <v>54</v>
+      </c>
+      <c r="C9" t="n">
+        <v>21.31578947368421</v>
       </c>
     </row>
     <row r="10">
@@ -996,7 +1025,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-141</v>
+        <v>141</v>
+      </c>
+      <c r="C10" t="n">
+        <v>55.65789473684211</v>
       </c>
     </row>
     <row r="11">
@@ -1006,7 +1038,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-59</v>
+        <v>59</v>
+      </c>
+      <c r="C11" t="n">
+        <v>23.28947368421053</v>
       </c>
     </row>
     <row r="12">
@@ -1016,7 +1051,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-51</v>
+        <v>51</v>
+      </c>
+      <c r="C12" t="n">
+        <v>20.13157894736842</v>
       </c>
     </row>
     <row r="13">
@@ -1026,7 +1064,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-28</v>
+        <v>28</v>
+      </c>
+      <c r="C13" t="n">
+        <v>11.05263157894737</v>
       </c>
     </row>
     <row r="14">
@@ -1036,7 +1077,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-66</v>
+        <v>66</v>
+      </c>
+      <c r="C14" t="n">
+        <v>26.05263157894737</v>
       </c>
     </row>
     <row r="15">
@@ -1046,7 +1090,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>-16</v>
+        <v>16</v>
+      </c>
+      <c r="C15" t="n">
+        <v>6.315789473684211</v>
       </c>
     </row>
     <row r="16">
@@ -1056,7 +1103,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-99</v>
+        <v>99</v>
+      </c>
+      <c r="C16" t="n">
+        <v>39.07894736842105</v>
       </c>
     </row>
     <row r="17">
@@ -1066,7 +1116,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-48</v>
+        <v>48</v>
+      </c>
+      <c r="C17" t="n">
+        <v>18.94736842105263</v>
       </c>
     </row>
     <row r="18">
@@ -1076,7 +1129,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-75</v>
+        <v>75</v>
+      </c>
+      <c r="C18" t="n">
+        <v>29.60526315789474</v>
       </c>
     </row>
     <row r="19">
@@ -1086,7 +1142,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-83</v>
+        <v>83</v>
+      </c>
+      <c r="C19" t="n">
+        <v>32.76315789473684</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added UPH and changed to positive in Single pick
</commit_message>
<xml_diff>
--- a/pick_counts.xlsx
+++ b/pick_counts.xlsx
@@ -768,7 +768,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -787,6 +787,11 @@
           <t>SinglePickQuantity</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>UPH</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -795,7 +800,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-27</v>
+        <v>27</v>
+      </c>
+      <c r="C2" t="n">
+        <v>11.40845070422535</v>
       </c>
     </row>
     <row r="3">
@@ -805,7 +813,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-10</v>
+        <v>10</v>
+      </c>
+      <c r="C3" t="n">
+        <v>4.225352112676056</v>
       </c>
     </row>
     <row r="4">
@@ -815,7 +826,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-23</v>
+        <v>23</v>
+      </c>
+      <c r="C4" t="n">
+        <v>9.71830985915493</v>
       </c>
     </row>
     <row r="5">
@@ -825,7 +839,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-35</v>
+        <v>35</v>
+      </c>
+      <c r="C5" t="n">
+        <v>14.7887323943662</v>
       </c>
     </row>
     <row r="6">
@@ -835,7 +852,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-44</v>
+        <v>44</v>
+      </c>
+      <c r="C6" t="n">
+        <v>18.59154929577465</v>
       </c>
     </row>
     <row r="7">
@@ -845,7 +865,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-60</v>
+        <v>60</v>
+      </c>
+      <c r="C7" t="n">
+        <v>25.35211267605634</v>
       </c>
     </row>
     <row r="8">
@@ -855,7 +878,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-72</v>
+        <v>72</v>
+      </c>
+      <c r="C8" t="n">
+        <v>30.4225352112676</v>
       </c>
     </row>
     <row r="9">
@@ -865,7 +891,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-98</v>
+        <v>98</v>
+      </c>
+      <c r="C9" t="n">
+        <v>41.40845070422535</v>
       </c>
     </row>
     <row r="10">
@@ -875,7 +904,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-50</v>
+        <v>50</v>
+      </c>
+      <c r="C10" t="n">
+        <v>21.12676056338028</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Total idle time after 15 mins
</commit_message>
<xml_diff>
--- a/pick_counts.xlsx
+++ b/pick_counts.xlsx
@@ -12,7 +12,8 @@
     <sheet name="REGULAR PICK" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="SINGLE PICK" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="REPLENISHMENT PICK" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Total Units picked by hour" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="IDLE TIME" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Total Units picked by hour" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -803,7 +804,7 @@
         <v>27</v>
       </c>
       <c r="C2" t="n">
-        <v>11.40845070422535</v>
+        <v>9.585798816568047</v>
       </c>
     </row>
     <row r="3">
@@ -816,7 +817,7 @@
         <v>10</v>
       </c>
       <c r="C3" t="n">
-        <v>4.225352112676056</v>
+        <v>3.550295857988166</v>
       </c>
     </row>
     <row r="4">
@@ -829,7 +830,7 @@
         <v>23</v>
       </c>
       <c r="C4" t="n">
-        <v>9.71830985915493</v>
+        <v>8.165680473372781</v>
       </c>
     </row>
     <row r="5">
@@ -842,7 +843,7 @@
         <v>35</v>
       </c>
       <c r="C5" t="n">
-        <v>14.7887323943662</v>
+        <v>12.42603550295858</v>
       </c>
     </row>
     <row r="6">
@@ -855,7 +856,7 @@
         <v>44</v>
       </c>
       <c r="C6" t="n">
-        <v>18.59154929577465</v>
+        <v>15.62130177514793</v>
       </c>
     </row>
     <row r="7">
@@ -868,7 +869,7 @@
         <v>60</v>
       </c>
       <c r="C7" t="n">
-        <v>25.35211267605634</v>
+        <v>21.30177514792899</v>
       </c>
     </row>
     <row r="8">
@@ -881,7 +882,7 @@
         <v>72</v>
       </c>
       <c r="C8" t="n">
-        <v>30.4225352112676</v>
+        <v>25.56213017751479</v>
       </c>
     </row>
     <row r="9">
@@ -894,7 +895,7 @@
         <v>98</v>
       </c>
       <c r="C9" t="n">
-        <v>41.40845070422535</v>
+        <v>34.79289940828402</v>
       </c>
     </row>
     <row r="10">
@@ -907,7 +908,7 @@
         <v>50</v>
       </c>
       <c r="C10" t="n">
-        <v>21.12676056338028</v>
+        <v>17.75147928994083</v>
       </c>
     </row>
   </sheetData>
@@ -956,7 +957,7 @@
         <v>64</v>
       </c>
       <c r="C2" t="n">
-        <v>25.26315789473684</v>
+        <v>22.72189349112426</v>
       </c>
     </row>
     <row r="3">
@@ -969,7 +970,7 @@
         <v>60</v>
       </c>
       <c r="C3" t="n">
-        <v>23.68421052631579</v>
+        <v>21.30177514792899</v>
       </c>
     </row>
     <row r="4">
@@ -982,7 +983,7 @@
         <v>89</v>
       </c>
       <c r="C4" t="n">
-        <v>35.13157894736842</v>
+        <v>31.59763313609467</v>
       </c>
     </row>
     <row r="5">
@@ -995,7 +996,7 @@
         <v>90</v>
       </c>
       <c r="C5" t="n">
-        <v>35.52631578947368</v>
+        <v>31.95266272189349</v>
       </c>
     </row>
     <row r="6">
@@ -1008,7 +1009,7 @@
         <v>48</v>
       </c>
       <c r="C6" t="n">
-        <v>18.94736842105263</v>
+        <v>17.04142011834319</v>
       </c>
     </row>
     <row r="7">
@@ -1021,7 +1022,7 @@
         <v>38</v>
       </c>
       <c r="C7" t="n">
-        <v>15</v>
+        <v>13.49112426035503</v>
       </c>
     </row>
     <row r="8">
@@ -1034,7 +1035,7 @@
         <v>76</v>
       </c>
       <c r="C8" t="n">
-        <v>30</v>
+        <v>26.98224852071006</v>
       </c>
     </row>
     <row r="9">
@@ -1047,7 +1048,7 @@
         <v>54</v>
       </c>
       <c r="C9" t="n">
-        <v>21.31578947368421</v>
+        <v>19.17159763313609</v>
       </c>
     </row>
     <row r="10">
@@ -1060,7 +1061,7 @@
         <v>141</v>
       </c>
       <c r="C10" t="n">
-        <v>55.65789473684211</v>
+        <v>50.05917159763313</v>
       </c>
     </row>
     <row r="11">
@@ -1073,7 +1074,7 @@
         <v>59</v>
       </c>
       <c r="C11" t="n">
-        <v>23.28947368421053</v>
+        <v>20.94674556213018</v>
       </c>
     </row>
     <row r="12">
@@ -1086,7 +1087,7 @@
         <v>51</v>
       </c>
       <c r="C12" t="n">
-        <v>20.13157894736842</v>
+        <v>18.10650887573964</v>
       </c>
     </row>
     <row r="13">
@@ -1099,7 +1100,7 @@
         <v>28</v>
       </c>
       <c r="C13" t="n">
-        <v>11.05263157894737</v>
+        <v>9.940828402366863</v>
       </c>
     </row>
     <row r="14">
@@ -1112,7 +1113,7 @@
         <v>66</v>
       </c>
       <c r="C14" t="n">
-        <v>26.05263157894737</v>
+        <v>23.43195266272189</v>
       </c>
     </row>
     <row r="15">
@@ -1125,7 +1126,7 @@
         <v>16</v>
       </c>
       <c r="C15" t="n">
-        <v>6.315789473684211</v>
+        <v>5.680473372781065</v>
       </c>
     </row>
     <row r="16">
@@ -1138,7 +1139,7 @@
         <v>99</v>
       </c>
       <c r="C16" t="n">
-        <v>39.07894736842105</v>
+        <v>35.14792899408284</v>
       </c>
     </row>
     <row r="17">
@@ -1151,7 +1152,7 @@
         <v>48</v>
       </c>
       <c r="C17" t="n">
-        <v>18.94736842105263</v>
+        <v>17.04142011834319</v>
       </c>
     </row>
     <row r="18">
@@ -1164,7 +1165,7 @@
         <v>75</v>
       </c>
       <c r="C18" t="n">
-        <v>29.60526315789474</v>
+        <v>26.62721893491124</v>
       </c>
     </row>
     <row r="19">
@@ -1177,7 +1178,7 @@
         <v>83</v>
       </c>
       <c r="C19" t="n">
-        <v>32.76315789473684</v>
+        <v>29.46745562130177</v>
       </c>
     </row>
   </sheetData>
@@ -1186,6 +1187,307 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>UserID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>TotalIdleTime</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ADOL798N.SEEMANNVAZQ</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>AGNE8120.CARUTH</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ALMER.VILLAMIN</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>BOHD0676.KUSHLIAK</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>BUDD0680.TENNAKOON</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>DEEP7013.KUMAR</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>DEVI789.SINGH</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>DIAN4065.ENTRIALGO</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>IREN797N.CABRERA</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>JEEW9554.SITUMUDALIG</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>JIGN776N.PATEL</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>KADE3054.ZONGO</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>LOWRHY-OTIENO.JAOKO</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>MELA6559.ROCHETTE</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>MICA0432.RIZKALLAMAR</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>NESR2403.ATTALAH</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>PATR5027.AMEH</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>STAN9294.BAUER</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>SURESH.DHAWAN</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>TANI2739.HOSSAINISLA</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>THIE6554.DIALLO</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>WESL5337.CADETTE</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>WILDINE.JEUNE</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>XUAN754N.LU</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>XYZE1559.MACASIL</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>YATI0689.YATIN</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>ZAKI0190.PHILLIPHORS</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1234,10 +1536,10 @@
         <v>-78</v>
       </c>
       <c r="C2" t="n">
-        <v>-101</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>-331</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
         <v>-39</v>
@@ -1251,10 +1553,10 @@
         <v>-126</v>
       </c>
       <c r="C3" t="n">
-        <v>-194</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>-432</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
         <v>-153</v>
@@ -1268,10 +1570,10 @@
         <v>-25</v>
       </c>
       <c r="C4" t="n">
-        <v>-124</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>-422</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
         <v>-256</v>
@@ -1304,10 +1606,10 @@
         <v>-229</v>
       </c>
       <c r="C6" t="n">
-        <v>-419</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>-1185</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
         <v>-448</v>

</xml_diff>

<commit_message>
Fixed some bugs in hour picked total
</commit_message>
<xml_diff>
--- a/pick_counts.xlsx
+++ b/pick_counts.xlsx
@@ -437,7 +437,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,27 +465,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ADOL798N.SEEMANNVAZQ</t>
+          <t>AGNE8120.CARUTH</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>14.55621301775148</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>AGNE8120.CARUTH</t>
+          <t>AHME0710.JUBRAN</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="C3" t="n">
-        <v>0.3550295857988165</v>
+        <v>23.7</v>
       </c>
     </row>
     <row r="4">
@@ -495,10 +495,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C4" t="n">
-        <v>6.745562130177515</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="5">
@@ -508,62 +508,101 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>128</v>
+        <v>154</v>
       </c>
       <c r="C5" t="n">
-        <v>45.44378698224852</v>
+        <v>46.2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>STAN9294.BAUER</t>
+          <t>KADE3054.ZONGO</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C6" t="n">
-        <v>8.875739644970414</v>
+        <v>11.4</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>TANI2739.HOSSAINISLA</t>
+          <t>LOANA.MBONGO</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>86</v>
+        <v>4</v>
       </c>
       <c r="C7" t="n">
-        <v>30.53254437869822</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>THIE6554.DIALLO</t>
+          <t>MAKEDA.OLLIVIERRE</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>15.97633136094674</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>PATI2298.ATSIANGBE</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>3</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.8999999999999999</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>SURESH.DHAWAN</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>39</v>
+      </c>
+      <c r="C10" t="n">
+        <v>11.7</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>THIE6554.DIALLO</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>56</v>
+      </c>
+      <c r="C11" t="n">
+        <v>16.8</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
           <t>XUAN754N.LU</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>103</v>
-      </c>
-      <c r="C9" t="n">
-        <v>36.5680473372781</v>
+      <c r="B12" t="n">
+        <v>353</v>
+      </c>
+      <c r="C12" t="n">
+        <v>105.9</v>
       </c>
     </row>
   </sheetData>
@@ -577,7 +616,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -605,40 +644,40 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ALMER.VILLAMIN</t>
+          <t>ADOL798N.SEEMANNVAZQ</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C2" t="n">
-        <v>7.100591715976331</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BOHD0676.KUSHLIAK</t>
+          <t>AGNE8120.CARUTH</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="C3" t="n">
-        <v>18.46153846153846</v>
+        <v>9.9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>DEEP7013.KUMAR</t>
+          <t>BOHD0676.KUSHLIAK</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>98</v>
       </c>
       <c r="C4" t="n">
-        <v>0.3550295857988165</v>
+        <v>29.4</v>
       </c>
     </row>
     <row r="5">
@@ -648,10 +687,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>33</v>
+        <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>11.71597633136095</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="6">
@@ -661,10 +700,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="C6" t="n">
-        <v>2.130177514792899</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="7">
@@ -674,75 +713,75 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C7" t="n">
-        <v>7.455621301775148</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>LOWRHY-OTIENO.JAOKO</t>
+          <t>LOANA.MBONGO</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C8" t="n">
-        <v>0.7100591715976331</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MICA0432.RIZKALLAMAR</t>
+          <t>MAKEDA.OLLIVIERRE</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C9" t="n">
-        <v>4.260355029585798</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>PATR5027.AMEH</t>
+          <t>PATI2298.ATSIANGBE</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C10" t="n">
-        <v>3.905325443786982</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>TANI2739.HOSSAINISLA</t>
+          <t>PATR5027.AMEH</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="C11" t="n">
-        <v>8.875739644970414</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>THIE6554.DIALLO</t>
+          <t>WESL5337.CADETTE</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C12" t="n">
-        <v>5.325443786982248</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="13">
@@ -752,10 +791,23 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="C13" t="n">
-        <v>11.00591715976331</v>
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>ZAKI0190.PHILLIPHORS</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>12</v>
+      </c>
+      <c r="C14" t="n">
+        <v>3.6</v>
       </c>
     </row>
   </sheetData>
@@ -769,7 +821,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -797,27 +849,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ALMER.VILLAMIN</t>
+          <t>BUDD0680.TENNAKOON</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C2" t="n">
-        <v>9.585798816568047</v>
+        <v>8.699999999999999</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BUDD0680.TENNAKOON</t>
+          <t>JEEW9554.SITUMUDALIG</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="C3" t="n">
-        <v>3.550295857988166</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="4">
@@ -827,88 +879,75 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>23</v>
+        <v>90</v>
       </c>
       <c r="C4" t="n">
-        <v>8.165680473372781</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>PATR5027.AMEH</t>
+          <t>OMAR6689.KHAN</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="C5" t="n">
-        <v>12.42603550295858</v>
+        <v>20.7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>STAN9294.BAUER</t>
+          <t>PATR5027.AMEH</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="C6" t="n">
-        <v>15.62130177514793</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>WESL5337.CADETTE</t>
+          <t>PRINCE.FORSON</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>60</v>
+        <v>18</v>
       </c>
       <c r="C7" t="n">
-        <v>21.30177514792899</v>
+        <v>5.399999999999999</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>WILDINE.JEUNE</t>
+          <t>WESL5337.CADETTE</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="C8" t="n">
-        <v>25.56213017751479</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>XYZE1559.MACASIL</t>
+          <t>WILDINE.JEUNE</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="C9" t="n">
-        <v>34.79289940828402</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>ZAKI0190.PHILLIPHORS</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>50</v>
-      </c>
-      <c r="C10" t="n">
-        <v>17.75147928994083</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -922,7 +961,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -950,235 +989,261 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BUDD0680.TENNAKOON</t>
+          <t>AHME0710.JUBRAN</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="C2" t="n">
-        <v>22.72189349112426</v>
+        <v>9.299999999999999</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DEVI789.SINGH</t>
+          <t>BOHD0676.KUSHLIAK</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="C3" t="n">
-        <v>21.30177514792899</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>IREN797N.CABRERA</t>
+          <t>BUDD0680.TENNAKOON</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>89</v>
+        <v>40</v>
       </c>
       <c r="C4" t="n">
-        <v>31.59763313609467</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>JEEW9554.SITUMUDALIG</t>
+          <t>DEVI789.SINGH</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="C5" t="n">
-        <v>31.95266272189349</v>
+        <v>19.2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>JIGN776N.PATEL</t>
+          <t>DIAN4065.ENTRIALGO</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>48</v>
+        <v>119</v>
       </c>
       <c r="C6" t="n">
-        <v>17.04142011834319</v>
+        <v>35.7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>KADE3054.ZONGO</t>
+          <t>IREN797N.CABRERA</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="C7" t="n">
-        <v>13.49112426035503</v>
+        <v>20.4</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>LOWRHY-OTIENO.JAOKO</t>
+          <t>JEEW9554.SITUMUDALIG</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="C8" t="n">
-        <v>26.98224852071006</v>
+        <v>27.6</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MELA6559.ROCHETTE</t>
+          <t>JIGN776N.PATEL</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="C9" t="n">
-        <v>19.17159763313609</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>MICA0432.RIZKALLAMAR</t>
+          <t>KADE3054.ZONGO</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>141</v>
+        <v>71</v>
       </c>
       <c r="C10" t="n">
-        <v>50.05917159763313</v>
+        <v>21.3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>NESR2403.ATTALAH</t>
+          <t>LOWRHY-OTIENO.JAOKO</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="C11" t="n">
-        <v>20.94674556213018</v>
+        <v>11.7</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>PATR5027.AMEH</t>
+          <t>MICA0432.RIZKALLAMAR</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>51</v>
+        <v>171</v>
       </c>
       <c r="C12" t="n">
-        <v>18.10650887573964</v>
+        <v>51.3</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>STAN9294.BAUER</t>
+          <t>NESR2403.ATTALAH</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C13" t="n">
-        <v>9.940828402366863</v>
+        <v>6.899999999999999</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>SURESH.DHAWAN</t>
+          <t>OMAR6689.KHAN</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="C14" t="n">
-        <v>23.43195266272189</v>
+        <v>12.6</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>THIE6554.DIALLO</t>
+          <t>PATR5027.AMEH</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="C15" t="n">
-        <v>5.680473372781065</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>WESL5337.CADETTE</t>
+          <t>PRINCE.FORSON</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>99</v>
+        <v>35</v>
       </c>
       <c r="C16" t="n">
-        <v>35.14792899408284</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>WILDINE.JEUNE</t>
+          <t>THIE6554.DIALLO</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>48</v>
+        <v>94</v>
       </c>
       <c r="C17" t="n">
-        <v>17.04142011834319</v>
+        <v>28.2</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>YATI0689.YATIN</t>
+          <t>WESL5337.CADETTE</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="C18" t="n">
-        <v>26.62721893491124</v>
+        <v>11.4</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>WILDINE.JEUNE</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>40</v>
+      </c>
+      <c r="C19" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>YATI0689.YATIN</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>77</v>
+      </c>
+      <c r="C20" t="n">
+        <v>23.1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
           <t>ZAKI0190.PHILLIPHORS</t>
         </is>
       </c>
-      <c r="B19" t="n">
-        <v>83</v>
-      </c>
-      <c r="C19" t="n">
-        <v>29.46745562130177</v>
+      <c r="B21" t="n">
+        <v>149</v>
+      </c>
+      <c r="C21" t="n">
+        <v>44.7</v>
       </c>
     </row>
   </sheetData>
@@ -1219,7 +1284,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>110</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3">
@@ -1229,17 +1294,17 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>76</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ALMER.VILLAMIN</t>
+          <t>AHME0710.JUBRAN</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>99</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5">
@@ -1249,7 +1314,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6">
@@ -1259,77 +1324,77 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>62</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>DEEP7013.KUMAR</t>
+          <t>DEVI789.SINGH</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>80</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>DEVI789.SINGH</t>
+          <t>DIAN4065.ENTRIALGO</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>81</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>DIAN4065.ENTRIALGO</t>
+          <t>IREN797N.CABRERA</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>37</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>IREN797N.CABRERA</t>
+          <t>JEEW9554.SITUMUDALIG</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>39</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>JEEW9554.SITUMUDALIG</t>
+          <t>JIGN776N.PATEL</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>35</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>JIGN776N.PATEL</t>
+          <t>KADE3054.ZONGO</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>115</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>KADE3054.ZONGO</t>
+          <t>LOANA.MBONGO</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>68</v>
+        <v>196</v>
       </c>
     </row>
     <row r="14">
@@ -1339,17 +1404,17 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>MELA6559.ROCHETTE</t>
+          <t>MAKEDA.OLLIVIERRE</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>73</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16">
@@ -1359,7 +1424,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>53</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17">
@@ -1369,13 +1434,13 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>87</v>
+        <v>191</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>PATR5027.AMEH</t>
+          <t>OMAR6689.KHAN</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -1385,81 +1450,81 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>STAN9294.BAUER</t>
+          <t>PATI2298.ATSIANGBE</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>61</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>SURESH.DHAWAN</t>
+          <t>PATR5027.AMEH</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>99</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>TANI2739.HOSSAINISLA</t>
+          <t>PRINCE.FORSON</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>66</v>
+        <v>188</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>THIE6554.DIALLO</t>
+          <t>SURESH.DHAWAN</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>95</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>WESL5337.CADETTE</t>
+          <t>THIE6554.DIALLO</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>15</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>WILDINE.JEUNE</t>
+          <t>WESL5337.CADETTE</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>40</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>XUAN754N.LU</t>
+          <t>WILDINE.JEUNE</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>XYZE1559.MACASIL</t>
+          <t>XUAN754N.LU</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27">
@@ -1469,7 +1534,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>85</v>
+        <v>135</v>
       </c>
     </row>
     <row r="28">
@@ -1479,7 +1544,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>22</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1533,16 +1598,16 @@
         <v>20</v>
       </c>
       <c r="B2" t="n">
-        <v>-78</v>
+        <v>-18</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>-313</v>
       </c>
       <c r="E2" t="n">
-        <v>-39</v>
+        <v>-119</v>
       </c>
     </row>
     <row r="3">
@@ -1550,16 +1615,16 @@
         <v>21</v>
       </c>
       <c r="B3" t="n">
-        <v>-126</v>
+        <v>-78</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>-111</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>-413</v>
       </c>
       <c r="E3" t="n">
-        <v>-153</v>
+        <v>-18</v>
       </c>
     </row>
     <row r="4">
@@ -1567,16 +1632,16 @@
         <v>22</v>
       </c>
       <c r="B4" t="n">
-        <v>-25</v>
+        <v>-99</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>-232</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>-373</v>
       </c>
       <c r="E4" t="n">
-        <v>-256</v>
+        <v>-356</v>
       </c>
     </row>
     <row r="5">
@@ -1584,16 +1649,16 @@
         <v>23</v>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>-62</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>-115</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>-175</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>-247</v>
       </c>
     </row>
     <row r="6">
@@ -1603,16 +1668,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-229</v>
+        <v>-257</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>-463</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>-1274</v>
       </c>
       <c r="E6" t="n">
-        <v>-448</v>
+        <v>-740</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added total quick move to the project
</commit_message>
<xml_diff>
--- a/pick_counts.xlsx
+++ b/pick_counts.xlsx
@@ -12,8 +12,9 @@
     <sheet name="REGULAR PICK" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="SINGLE PICK" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="REPLENISHMENT PICK" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="IDLE TIME" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Total Units picked by hour" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="QUICK MOVE" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="IDLE TIME" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Total Units picked by hour" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -437,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,53 +466,53 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>AGNE8120.CARUTH</t>
+          <t>ADOL798N.SEEMANNVAZQ</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3</v>
+        <v>7.17948717948718</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>AHME0710.JUBRAN</t>
+          <t>BOHD0676.KUSHLIAK</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>79</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>23.7</v>
+        <v>0.2564102564102564</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>BOHD0676.KUSHLIAK</t>
+          <t>DIAN4065.ENTRIALGO</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>12</v>
+        <v>175</v>
       </c>
       <c r="C4" t="n">
-        <v>3.6</v>
+        <v>44.87179487179488</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>DIAN4065.ENTRIALGO</t>
+          <t>HARV952N.PANDHER</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>154</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>46.2</v>
+        <v>0.2564102564102564</v>
       </c>
     </row>
     <row r="6">
@@ -521,62 +522,62 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>11.4</v>
+        <v>0.2564102564102564</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>LOANA.MBONGO</t>
+          <t>MAKEDA.OLLIVIERRE</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C7" t="n">
-        <v>1.2</v>
+        <v>1.794871794871795</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MAKEDA.OLLIVIERRE</t>
+          <t>PATR5027.AMEH</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>0.3</v>
+        <v>0.2564102564102564</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>PATI2298.ATSIANGBE</t>
+          <t>RARG046N.YEBOAH</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="C9" t="n">
-        <v>0.8999999999999999</v>
+        <v>6.153846153846154</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>SURESH.DHAWAN</t>
+          <t>TANI2739.HOSSAINISLA</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>39</v>
+        <v>163</v>
       </c>
       <c r="C10" t="n">
-        <v>11.7</v>
+        <v>41.7948717948718</v>
       </c>
     </row>
     <row r="11">
@@ -586,10 +587,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>56</v>
+        <v>110</v>
       </c>
       <c r="C11" t="n">
-        <v>16.8</v>
+        <v>28.2051282051282</v>
       </c>
     </row>
     <row r="12">
@@ -599,10 +600,36 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>353</v>
+        <v>240</v>
       </c>
       <c r="C12" t="n">
-        <v>105.9</v>
+        <v>61.53846153846154</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>YATI0689.YATIN</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>3</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.7692307692307693</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>ZAHIDGUL.MINHAS</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.5128205128205129</v>
       </c>
     </row>
   </sheetData>
@@ -644,157 +671,157 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ADOL798N.SEEMANNVAZQ</t>
+          <t>AGNE8120.CARUTH</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="C2" t="n">
-        <v>12</v>
+        <v>1.794871794871795</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>AGNE8120.CARUTH</t>
+          <t>BOHD0676.KUSHLIAK</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>9.9</v>
+        <v>0.2564102564102564</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>BOHD0676.KUSHLIAK</t>
+          <t>DEVI789.SINGH</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>98</v>
+        <v>2</v>
       </c>
       <c r="C4" t="n">
-        <v>29.4</v>
+        <v>0.5128205128205129</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>DIAN4065.ENTRIALGO</t>
+          <t>HARV952N.PANDHER</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>0.8999999999999999</v>
+        <v>0.2564102564102564</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>IREN797N.CABRERA</t>
+          <t>KADE3054.ZONGO</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="C6" t="n">
-        <v>8.1</v>
+        <v>0.5128205128205129</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>JEEW9554.SITUMUDALIG</t>
+          <t>PATR5027.AMEH</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C7" t="n">
-        <v>3.3</v>
+        <v>0.5128205128205129</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>LOANA.MBONGO</t>
+          <t>PRITTY.MAZUMDER</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>1.2</v>
+        <v>0.2564102564102564</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MAKEDA.OLLIVIERRE</t>
+          <t>STAN9294.BAUER</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C9" t="n">
-        <v>1.5</v>
+        <v>0.2564102564102564</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>PATI2298.ATSIANGBE</t>
+          <t>WESL5337.CADETTE</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>0.8999999999999999</v>
+        <v>0.2564102564102564</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>PATR5027.AMEH</t>
+          <t>WILDINE.JEUNE</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>0.8999999999999999</v>
+        <v>1.538461538461539</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>WESL5337.CADETTE</t>
+          <t>YATI0689.YATIN</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>0.8999999999999999</v>
+        <v>0.5128205128205129</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>XUAN754N.LU</t>
+          <t>ZAHIDGUL.MINHAS</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C13" t="n">
-        <v>4.5</v>
+        <v>0.2564102564102564</v>
       </c>
     </row>
     <row r="14">
@@ -804,10 +831,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C14" t="n">
-        <v>3.6</v>
+        <v>1.025641025641026</v>
       </c>
     </row>
   </sheetData>
@@ -821,7 +848,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -853,101 +880,205 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C2" t="n">
-        <v>8.699999999999999</v>
+        <v>10.25641025641026</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>JEEW9554.SITUMUDALIG</t>
+          <t>DEVI789.SINGH</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C3" t="n">
-        <v>8.1</v>
+        <v>6.153846153846154</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>LOWRHY-OTIENO.JAOKO</t>
+          <t>IREN797N.CABRERA</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>90</v>
+        <v>56</v>
       </c>
       <c r="C4" t="n">
-        <v>27</v>
+        <v>14.35897435897436</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>OMAR6689.KHAN</t>
+          <t>JEEW9554.SITUMUDALIG</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>69</v>
+        <v>130</v>
       </c>
       <c r="C5" t="n">
-        <v>20.7</v>
+        <v>33.33333333333334</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>PATR5027.AMEH</t>
+          <t>KADE3054.ZONGO</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="C6" t="n">
-        <v>18</v>
+        <v>6.923076923076923</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>PRINCE.FORSON</t>
+          <t>LOANA.MBONGO</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>18</v>
+        <v>125</v>
       </c>
       <c r="C7" t="n">
-        <v>5.399999999999999</v>
+        <v>32.05128205128205</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>WESL5337.CADETTE</t>
+          <t>LOWRHY-OTIENO.JAOKO</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="C8" t="n">
-        <v>27</v>
+        <v>24.61538461538462</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>MICA0432.RIZKALLAMAR</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>104</v>
+      </c>
+      <c r="C9" t="n">
+        <v>26.66666666666667</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>OMAR6689.KHAN</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>83</v>
+      </c>
+      <c r="C10" t="n">
+        <v>21.28205128205128</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>PATI2298.ATSIANGBE</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>17</v>
+      </c>
+      <c r="C11" t="n">
+        <v>4.358974358974359</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>RARG046N.YEBOAH</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>47</v>
+      </c>
+      <c r="C12" t="n">
+        <v>12.05128205128205</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>STAN9294.BAUER</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>19</v>
+      </c>
+      <c r="C13" t="n">
+        <v>4.871794871794872</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>WESL5337.CADETTE</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>72</v>
+      </c>
+      <c r="C14" t="n">
+        <v>18.46153846153846</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>WILDINE.JEUNE</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>80</v>
-      </c>
-      <c r="C9" t="n">
-        <v>24</v>
+      <c r="B15" t="n">
+        <v>36</v>
+      </c>
+      <c r="C15" t="n">
+        <v>9.230769230769232</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>YATI0689.YATIN</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>27</v>
+      </c>
+      <c r="C16" t="n">
+        <v>6.923076923076923</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>ZAKI0190.PHILLIPHORS</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>52</v>
+      </c>
+      <c r="C17" t="n">
+        <v>13.33333333333333</v>
       </c>
     </row>
   </sheetData>
@@ -961,7 +1092,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -989,66 +1120,66 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>AHME0710.JUBRAN</t>
+          <t>ANJALI.BAKSHI</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C2" t="n">
-        <v>9.299999999999999</v>
+        <v>5.641025641025641</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BOHD0676.KUSHLIAK</t>
+          <t>BUDD0680.TENNAKOON</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="C3" t="n">
-        <v>3.3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>BUDD0680.TENNAKOON</t>
+          <t>DEVI789.SINGH</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="C4" t="n">
-        <v>12</v>
+        <v>1.538461538461539</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>DEVI789.SINGH</t>
+          <t>DIAN4065.ENTRIALGO</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C5" t="n">
-        <v>19.2</v>
+        <v>14.61538461538461</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DIAN4065.ENTRIALGO</t>
+          <t>HARV952N.PANDHER</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>119</v>
+        <v>16</v>
       </c>
       <c r="C6" t="n">
-        <v>35.7</v>
+        <v>4.102564102564103</v>
       </c>
     </row>
     <row r="7">
@@ -1058,192 +1189,244 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>68</v>
+        <v>110</v>
       </c>
       <c r="C7" t="n">
-        <v>20.4</v>
+        <v>28.2051282051282</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>JEEW9554.SITUMUDALIG</t>
+          <t>JIGN776N.PATEL</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>92</v>
+        <v>40</v>
       </c>
       <c r="C8" t="n">
-        <v>27.6</v>
+        <v>10.25641025641026</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>JIGN776N.PATEL</t>
+          <t>KADE3054.ZONGO</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="C9" t="n">
-        <v>7.5</v>
+        <v>9.487179487179487</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>KADE3054.ZONGO</t>
+          <t>LOWRHY-OTIENO.JAOKO</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C10" t="n">
-        <v>21.3</v>
+        <v>19.48717948717949</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>LOWRHY-OTIENO.JAOKO</t>
+          <t>MICA0432.RIZKALLAMAR</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>39</v>
+        <v>128</v>
       </c>
       <c r="C11" t="n">
-        <v>11.7</v>
+        <v>32.82051282051282</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>MICA0432.RIZKALLAMAR</t>
+          <t>NESR2403.ATTALAH</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>171</v>
+        <v>7</v>
       </c>
       <c r="C12" t="n">
-        <v>51.3</v>
+        <v>1.794871794871795</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>NESR2403.ATTALAH</t>
+          <t>OMAR6689.KHAN</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C13" t="n">
-        <v>6.899999999999999</v>
+        <v>4.358974358974359</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>OMAR6689.KHAN</t>
+          <t>PATI2298.ATSIANGBE</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C14" t="n">
-        <v>12.6</v>
+        <v>13.58974358974359</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>PATR5027.AMEH</t>
+          <t>PRITTY.MAZUMDER</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="C15" t="n">
-        <v>13.5</v>
+        <v>4.102564102564103</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>PRINCE.FORSON</t>
+          <t>RARG046N.YEBOAH</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C16" t="n">
-        <v>10.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>THIE6554.DIALLO</t>
+          <t>RFBASE</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>94</v>
+        <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>28.2</v>
+        <v>4.102564102564103</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>WESL5337.CADETTE</t>
+          <t>STAN9294.BAUER</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="C18" t="n">
-        <v>11.4</v>
+        <v>1.538461538461539</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>WILDINE.JEUNE</t>
+          <t>TANI2739.HOSSAINISLA</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="C19" t="n">
-        <v>12</v>
+        <v>15.8974358974359</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>YATI0689.YATIN</t>
+          <t>THIE6554.DIALLO</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C20" t="n">
-        <v>23.1</v>
+        <v>17.43589743589744</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>WESL5337.CADETTE</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>50</v>
+      </c>
+      <c r="C21" t="n">
+        <v>12.82051282051282</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>WILDINE.JEUNE</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>78</v>
+      </c>
+      <c r="C22" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>XUAN754N.LU</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>23</v>
+      </c>
+      <c r="C23" t="n">
+        <v>5.897435897435898</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>YATI0689.YATIN</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>18</v>
+      </c>
+      <c r="C24" t="n">
+        <v>4.615384615384616</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
           <t>ZAKI0190.PHILLIPHORS</t>
         </is>
       </c>
-      <c r="B21" t="n">
-        <v>149</v>
-      </c>
-      <c r="C21" t="n">
-        <v>44.7</v>
+      <c r="B25" t="n">
+        <v>70</v>
+      </c>
+      <c r="C25" t="n">
+        <v>17.94871794871795</v>
       </c>
     </row>
   </sheetData>
@@ -1257,7 +1440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1273,7 +1456,12 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>TotalIdleTime</t>
+          <t>QuickMoveQuantity</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>UPH</t>
         </is>
       </c>
     </row>
@@ -1284,267 +1472,166 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>159</v>
+        <v>28</v>
+      </c>
+      <c r="C2" t="n">
+        <v>7.17948717948718</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>AGNE8120.CARUTH</t>
+          <t>BOHD0676.KUSHLIAK</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>181</v>
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.2564102564102564</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>AHME0710.JUBRAN</t>
+          <t>DIAN4065.ENTRIALGO</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>151</v>
+        <v>175</v>
+      </c>
+      <c r="C4" t="n">
+        <v>44.87179487179488</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>BOHD0676.KUSHLIAK</t>
+          <t>HARV952N.PANDHER</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>63</v>
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.2564102564102564</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>BUDD0680.TENNAKOON</t>
+          <t>KADE3054.ZONGO</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>114</v>
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.2564102564102564</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>DEVI789.SINGH</t>
+          <t>MAKEDA.OLLIVIERRE</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>116</v>
+        <v>4</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1.025641025641026</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>DIAN4065.ENTRIALGO</t>
+          <t>PATR5027.AMEH</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>54</v>
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.2564102564102564</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>IREN797N.CABRERA</t>
+          <t>RARG046N.YEBOAH</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>80</v>
+        <v>24</v>
+      </c>
+      <c r="C9" t="n">
+        <v>6.153846153846154</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>JEEW9554.SITUMUDALIG</t>
+          <t>TANI2739.HOSSAINISLA</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>71</v>
+        <v>163</v>
+      </c>
+      <c r="C10" t="n">
+        <v>41.7948717948718</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>JIGN776N.PATEL</t>
+          <t>THIE6554.DIALLO</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>122</v>
+        <v>110</v>
+      </c>
+      <c r="C11" t="n">
+        <v>28.2051282051282</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>KADE3054.ZONGO</t>
+          <t>XUAN754N.LU</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>101</v>
+        <v>240</v>
+      </c>
+      <c r="C12" t="n">
+        <v>61.53846153846154</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>LOANA.MBONGO</t>
+          <t>YATI0689.YATIN</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>196</v>
+        <v>3</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.7692307692307693</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>LOWRHY-OTIENO.JAOKO</t>
+          <t>ZAHIDGUL.MINHAS</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>MAKEDA.OLLIVIERRE</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>MICA0432.RIZKALLAMAR</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>NESR2403.ATTALAH</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>OMAR6689.KHAN</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>PATI2298.ATSIANGBE</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>PATR5027.AMEH</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>PRINCE.FORSON</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>SURESH.DHAWAN</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>THIE6554.DIALLO</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>WESL5337.CADETTE</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>WILDINE.JEUNE</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>XUAN754N.LU</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>YATI0689.YATIN</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>ZAKI0190.PHILLIPHORS</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>49</v>
+        <v>1</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.2564102564102564</v>
       </c>
     </row>
   </sheetData>
@@ -1553,6 +1640,357 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>UserID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>TotalIdleTime</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ADOL798N.SEEMANNVAZQ</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>AGNE8120.CARUTH</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ANJALI.BAKSHI</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>BOHD0676.KUSHLIAK</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>BUDD0680.TENNAKOON</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>DEVI789.SINGH</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>DIAN4065.ENTRIALGO</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>HARV952N.PANDHER</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>IREN797N.CABRERA</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>JEEW9554.SITUMUDALIG</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>JIGN776N.PATEL</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>KADE3054.ZONGO</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>LOANA.MBONGO</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>LOWRHY-OTIENO.JAOKO</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>MAKEDA.OLLIVIERRE</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>MICA0432.RIZKALLAMAR</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>NESR2403.ATTALAH</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>OMAR6689.KHAN</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>PATI2298.ATSIANGBE</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>PATR5027.AMEH</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>PRITTY.MAZUMDER</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>RARG046N.YEBOAH</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>RFBASE</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>STAN9294.BAUER</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>TANI2739.HOSSAINISLA</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>THIE6554.DIALLO</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>WESL5337.CADETTE</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>WILDINE.JEUNE</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>XUAN754N.LU</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>YATI0689.YATIN</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>ZAHIDGUL.MINHAS</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>ZAKI0190.PHILLIPHORS</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1598,16 +2036,16 @@
         <v>20</v>
       </c>
       <c r="B2" t="n">
-        <v>-18</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>-5</v>
+        <v>-25</v>
       </c>
       <c r="D2" t="n">
-        <v>-313</v>
+        <v>-442</v>
       </c>
       <c r="E2" t="n">
-        <v>-119</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="3">
@@ -1615,16 +2053,16 @@
         <v>21</v>
       </c>
       <c r="B3" t="n">
-        <v>-78</v>
+        <v>-5</v>
       </c>
       <c r="C3" t="n">
-        <v>-111</v>
+        <v>-264</v>
       </c>
       <c r="D3" t="n">
-        <v>-413</v>
+        <v>-349</v>
       </c>
       <c r="E3" t="n">
-        <v>-18</v>
+        <v>-95</v>
       </c>
     </row>
     <row r="4">
@@ -1632,16 +2070,16 @@
         <v>22</v>
       </c>
       <c r="B4" t="n">
-        <v>-99</v>
+        <v>-9</v>
       </c>
       <c r="C4" t="n">
-        <v>-232</v>
+        <v>-353</v>
       </c>
       <c r="D4" t="n">
-        <v>-373</v>
+        <v>-229</v>
       </c>
       <c r="E4" t="n">
-        <v>-356</v>
+        <v>-320</v>
       </c>
     </row>
     <row r="5">
@@ -1649,16 +2087,16 @@
         <v>23</v>
       </c>
       <c r="B5" t="n">
-        <v>-62</v>
+        <v>-17</v>
       </c>
       <c r="C5" t="n">
-        <v>-115</v>
+        <v>-313</v>
       </c>
       <c r="D5" t="n">
-        <v>-175</v>
+        <v>-34</v>
       </c>
       <c r="E5" t="n">
-        <v>-247</v>
+        <v>-334</v>
       </c>
     </row>
     <row r="6">
@@ -1668,16 +2106,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-257</v>
+        <v>-31</v>
       </c>
       <c r="C6" t="n">
-        <v>-463</v>
+        <v>-955</v>
       </c>
       <c r="D6" t="n">
-        <v>-1274</v>
+        <v>-1054</v>
       </c>
       <c r="E6" t="n">
-        <v>-740</v>
+        <v>-756</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected quick move code and fixed idle time code
</commit_message>
<xml_diff>
--- a/pick_counts.xlsx
+++ b/pick_counts.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,170 +466,92 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ADOL798N.SEEMANNVAZQ</t>
+          <t>BOHD0676.KUSHLIAK</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C2" t="n">
-        <v>7.17948717948718</v>
+        <v>11.70731707317073</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BOHD0676.KUSHLIAK</t>
+          <t>DIAN4065.ENTRIALGO</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>77</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2564102564102564</v>
+        <v>28.17073170731707</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>DIAN4065.ENTRIALGO</t>
+          <t>PATI2298.ATSIANGBE</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>175</v>
+        <v>14</v>
       </c>
       <c r="C4" t="n">
-        <v>44.87179487179488</v>
+        <v>5.121951219512195</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>HARV952N.PANDHER</t>
+          <t>RAMI9087.SAIHI</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2564102564102564</v>
+        <v>16.82926829268293</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>KADE3054.ZONGO</t>
+          <t>TANI2739.HOSSAINISLA</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="C6" t="n">
-        <v>0.2564102564102564</v>
+        <v>21.58536585365854</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MAKEDA.OLLIVIERRE</t>
+          <t>THIE6554.DIALLO</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="C7" t="n">
-        <v>1.794871794871795</v>
+        <v>16.82926829268293</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>PATR5027.AMEH</t>
+          <t>XUAN754N.LU</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>72</v>
       </c>
       <c r="C8" t="n">
-        <v>0.2564102564102564</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>RARG046N.YEBOAH</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>24</v>
-      </c>
-      <c r="C9" t="n">
-        <v>6.153846153846154</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>TANI2739.HOSSAINISLA</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>163</v>
-      </c>
-      <c r="C10" t="n">
-        <v>41.7948717948718</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>THIE6554.DIALLO</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>110</v>
-      </c>
-      <c r="C11" t="n">
-        <v>28.2051282051282</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>XUAN754N.LU</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>240</v>
-      </c>
-      <c r="C12" t="n">
-        <v>61.53846153846154</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>YATI0689.YATIN</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>3</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.7692307692307693</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>ZAHIDGUL.MINHAS</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>2</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0.5128205128205129</v>
+        <v>26.34146341463414</v>
       </c>
     </row>
   </sheetData>
@@ -643,7 +565,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -671,170 +593,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>AGNE8120.CARUTH</t>
+          <t>TANI2739.HOSSAINISLA</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>1.794871794871795</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>BOHD0676.KUSHLIAK</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.2564102564102564</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>DEVI789.SINGH</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.5128205128205129</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>HARV952N.PANDHER</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.2564102564102564</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>KADE3054.ZONGO</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>2</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.5128205128205129</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>PATR5027.AMEH</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>2</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.5128205128205129</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>PRITTY.MAZUMDER</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.2564102564102564</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>STAN9294.BAUER</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.2564102564102564</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>WESL5337.CADETTE</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>1</v>
-      </c>
-      <c r="C10" t="n">
-        <v>0.2564102564102564</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>WILDINE.JEUNE</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>6</v>
-      </c>
-      <c r="C11" t="n">
-        <v>1.538461538461539</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>YATI0689.YATIN</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>2</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0.5128205128205129</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>ZAHIDGUL.MINHAS</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.2564102564102564</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>ZAKI0190.PHILLIPHORS</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>4</v>
-      </c>
-      <c r="C14" t="n">
-        <v>1.025641025641026</v>
+        <v>0.3658536585365854</v>
       </c>
     </row>
   </sheetData>
@@ -848,7 +614,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -876,209 +642,118 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BUDD0680.TENNAKOON</t>
+          <t>BOHD0676.KUSHLIAK</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="C2" t="n">
-        <v>10.25641025641026</v>
+        <v>19.02439024390244</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DEVI789.SINGH</t>
+          <t>JEEW9554.SITUMUDALIG</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>6.153846153846154</v>
+        <v>1.829268292682927</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>IREN797N.CABRERA</t>
+          <t>OMAR6689.KHAN</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="C4" t="n">
-        <v>14.35897435897436</v>
+        <v>8.780487804878049</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>JEEW9554.SITUMUDALIG</t>
+          <t>RAMI9087.SAIHI</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>130</v>
+        <v>23</v>
       </c>
       <c r="C5" t="n">
-        <v>33.33333333333334</v>
+        <v>8.414634146341463</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>KADE3054.ZONGO</t>
+          <t>TANI2739.HOSSAINISLA</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C6" t="n">
-        <v>6.923076923076923</v>
+        <v>6.219512195121951</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>LOANA.MBONGO</t>
+          <t>THIE6554.DIALLO</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>125</v>
+        <v>72</v>
       </c>
       <c r="C7" t="n">
-        <v>32.05128205128205</v>
+        <v>26.34146341463414</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>LOWRHY-OTIENO.JAOKO</t>
+          <t>WESL5337.CADETTE</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>96</v>
+        <v>13</v>
       </c>
       <c r="C8" t="n">
-        <v>24.61538461538462</v>
+        <v>4.75609756097561</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MICA0432.RIZKALLAMAR</t>
+          <t>XUAN754N.LU</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>104</v>
+        <v>46</v>
       </c>
       <c r="C9" t="n">
-        <v>26.66666666666667</v>
+        <v>16.82926829268293</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>OMAR6689.KHAN</t>
+          <t>ZAHIDGUL.MINHAS</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C10" t="n">
-        <v>21.28205128205128</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>PATI2298.ATSIANGBE</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>17</v>
-      </c>
-      <c r="C11" t="n">
-        <v>4.358974358974359</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>RARG046N.YEBOAH</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>47</v>
-      </c>
-      <c r="C12" t="n">
-        <v>12.05128205128205</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>STAN9294.BAUER</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>19</v>
-      </c>
-      <c r="C13" t="n">
-        <v>4.871794871794872</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>WESL5337.CADETTE</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>72</v>
-      </c>
-      <c r="C14" t="n">
-        <v>18.46153846153846</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>WILDINE.JEUNE</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>36</v>
-      </c>
-      <c r="C15" t="n">
-        <v>9.230769230769232</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>YATI0689.YATIN</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>27</v>
-      </c>
-      <c r="C16" t="n">
-        <v>6.923076923076923</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>ZAKI0190.PHILLIPHORS</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>52</v>
-      </c>
-      <c r="C17" t="n">
-        <v>13.33333333333333</v>
+        <v>29.63414634146341</v>
       </c>
     </row>
   </sheetData>
@@ -1092,7 +767,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1120,14 +795,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ANJALI.BAKSHI</t>
+          <t>BOHD0676.KUSHLIAK</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C2" t="n">
-        <v>5.641025641025641</v>
+        <v>3.292682926829268</v>
       </c>
     </row>
     <row r="3">
@@ -1137,296 +812,218 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="C3" t="n">
-        <v>10</v>
+        <v>4.024390243902439</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>DEVI789.SINGH</t>
+          <t>IREN797N.CABRERA</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="C4" t="n">
-        <v>1.538461538461539</v>
+        <v>21.58536585365854</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>DIAN4065.ENTRIALGO</t>
+          <t>JEEW9554.SITUMUDALIG</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="C5" t="n">
-        <v>14.61538461538461</v>
+        <v>11.34146341463415</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>HARV952N.PANDHER</t>
+          <t>KADE3054.ZONGO</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C6" t="n">
-        <v>4.102564102564103</v>
+        <v>9.146341463414634</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>IREN797N.CABRERA</t>
+          <t>LOANA.MBONGO</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>110</v>
+        <v>56</v>
       </c>
       <c r="C7" t="n">
-        <v>28.2051282051282</v>
+        <v>20.48780487804878</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>JIGN776N.PATEL</t>
+          <t>LOWRHY-OTIENO.JAOKO</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="C8" t="n">
-        <v>10.25641025641026</v>
+        <v>8.048780487804878</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>KADE3054.ZONGO</t>
+          <t>MICA0432.RIZKALLAMAR</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C9" t="n">
-        <v>9.487179487179487</v>
+        <v>19.75609756097561</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>LOWRHY-OTIENO.JAOKO</t>
+          <t>OMAR6689.KHAN</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="C10" t="n">
-        <v>19.48717948717949</v>
+        <v>12.80487804878049</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>MICA0432.RIZKALLAMAR</t>
+          <t>RAMI9087.SAIHI</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>128</v>
+        <v>17</v>
       </c>
       <c r="C11" t="n">
-        <v>32.82051282051282</v>
+        <v>6.219512195121951</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>NESR2403.ATTALAH</t>
+          <t>RARG046N.YEBOAH</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C12" t="n">
-        <v>1.794871794871795</v>
+        <v>7.317073170731708</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>OMAR6689.KHAN</t>
+          <t>STAN9294.BAUER</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C13" t="n">
-        <v>4.358974358974359</v>
+        <v>2.560975609756098</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>PATI2298.ATSIANGBE</t>
+          <t>THIE6554.DIALLO</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="C14" t="n">
-        <v>13.58974358974359</v>
+        <v>4.390243902439025</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>PRITTY.MAZUMDER</t>
+          <t>WESL5337.CADETTE</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="C15" t="n">
-        <v>4.102564102564103</v>
+        <v>10.97560975609756</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>RARG046N.YEBOAH</t>
+          <t>WILDINE.JEUNE</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C16" t="n">
-        <v>10</v>
+        <v>9.512195121951219</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>RFBASE</t>
+          <t>XUAN754N.LU</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C17" t="n">
-        <v>4.102564102564103</v>
+        <v>1.463414634146341</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>STAN9294.BAUER</t>
+          <t>ZAHIDGUL.MINHAS</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="C18" t="n">
-        <v>1.538461538461539</v>
+        <v>11.70731707317073</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>TANI2739.HOSSAINISLA</t>
+          <t>ZAKI0190.PHILLIPHORS</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="C19" t="n">
-        <v>15.8974358974359</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>THIE6554.DIALLO</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>68</v>
-      </c>
-      <c r="C20" t="n">
-        <v>17.43589743589744</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>WESL5337.CADETTE</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>50</v>
-      </c>
-      <c r="C21" t="n">
-        <v>12.82051282051282</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>WILDINE.JEUNE</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>78</v>
-      </c>
-      <c r="C22" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>XUAN754N.LU</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>23</v>
-      </c>
-      <c r="C23" t="n">
-        <v>5.897435897435898</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>YATI0689.YATIN</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>18</v>
-      </c>
-      <c r="C24" t="n">
-        <v>4.615384615384616</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>ZAKI0190.PHILLIPHORS</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>70</v>
-      </c>
-      <c r="C25" t="n">
-        <v>17.94871794871795</v>
+        <v>11.70731707317073</v>
       </c>
     </row>
   </sheetData>
@@ -1440,7 +1037,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1468,170 +1065,79 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ADOL798N.SEEMANNVAZQ</t>
+          <t>BOHD0676.KUSHLIAK</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>28</v>
+        <v>89</v>
       </c>
       <c r="C2" t="n">
-        <v>7.17948717948718</v>
+        <v>32.5609756097561</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BOHD0676.KUSHLIAK</t>
+          <t>OMAR6689.KHAN</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2564102564102564</v>
+        <v>3.658536585365854</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>DIAN4065.ENTRIALGO</t>
+          <t>RAMI9087.SAIHI</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>175</v>
+        <v>40</v>
       </c>
       <c r="C4" t="n">
-        <v>44.87179487179488</v>
+        <v>14.63414634146342</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>HARV952N.PANDHER</t>
+          <t>TANI2739.HOSSAINISLA</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C5" t="n">
-        <v>0.2564102564102564</v>
+        <v>6.951219512195122</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>KADE3054.ZONGO</t>
+          <t>THIE6554.DIALLO</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="C6" t="n">
-        <v>0.2564102564102564</v>
+        <v>21.58536585365854</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MAKEDA.OLLIVIERRE</t>
+          <t>XUAN754N.LU</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>4</v>
       </c>
       <c r="C7" t="n">
-        <v>1.025641025641026</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>PATR5027.AMEH</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0.2564102564102564</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>RARG046N.YEBOAH</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>24</v>
-      </c>
-      <c r="C9" t="n">
-        <v>6.153846153846154</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>TANI2739.HOSSAINISLA</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>163</v>
-      </c>
-      <c r="C10" t="n">
-        <v>41.7948717948718</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>THIE6554.DIALLO</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>110</v>
-      </c>
-      <c r="C11" t="n">
-        <v>28.2051282051282</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>XUAN754N.LU</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>240</v>
-      </c>
-      <c r="C12" t="n">
-        <v>61.53846153846154</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>YATI0689.YATIN</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>3</v>
-      </c>
-      <c r="C13" t="n">
-        <v>0.7692307692307693</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>ZAHIDGUL.MINHAS</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0.2564102564102564</v>
+        <v>1.463414634146341</v>
       </c>
     </row>
   </sheetData>
@@ -1645,7 +1151,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1668,321 +1174,211 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ADOL798N.SEEMANNVAZQ</t>
+          <t>BOHD0676.KUSHLIAK</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>66</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>AGNE8120.CARUTH</t>
+          <t>BUDD0680.TENNAKOON</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>142</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ANJALI.BAKSHI</t>
+          <t>DIAN4065.ENTRIALGO</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>84</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>BOHD0676.KUSHLIAK</t>
+          <t>IREN797N.CABRERA</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>101</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>BUDD0680.TENNAKOON</t>
+          <t>JEEW9554.SITUMUDALIG</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>96</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>DEVI789.SINGH</t>
+          <t>KADE3054.ZONGO</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>217</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>DIAN4065.ENTRIALGO</t>
+          <t>LOANA.MBONGO</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>114</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>HARV952N.PANDHER</t>
+          <t>LOWRHY-OTIENO.JAOKO</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>205</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>IREN797N.CABRERA</t>
+          <t>MICA0432.RIZKALLAMAR</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>57</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>JEEW9554.SITUMUDALIG</t>
+          <t>OMAR6689.KHAN</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>21</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>JIGN776N.PATEL</t>
+          <t>PATI2298.ATSIANGBE</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>132</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>KADE3054.ZONGO</t>
+          <t>RAMI9087.SAIHI</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>115</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>LOANA.MBONGO</t>
+          <t>RARG046N.YEBOAH</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>112</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>LOWRHY-OTIENO.JAOKO</t>
+          <t>STAN9294.BAUER</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>63</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>MAKEDA.OLLIVIERRE</t>
+          <t>TANI2739.HOSSAINISLA</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>130</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>MICA0432.RIZKALLAMAR</t>
+          <t>THIE6554.DIALLO</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>NESR2403.ATTALAH</t>
+          <t>WESL5337.CADETTE</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>152</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>OMAR6689.KHAN</t>
+          <t>WILDINE.JEUNE</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>51</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>PATI2298.ATSIANGBE</t>
+          <t>XUAN754N.LU</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>PATR5027.AMEH</t>
+          <t>ZAHIDGUL.MINHAS</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>192</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>PRITTY.MAZUMDER</t>
+          <t>ZAKI0190.PHILLIPHORS</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>RARG046N.YEBOAH</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>RFBASE</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>STAN9294.BAUER</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>TANI2739.HOSSAINISLA</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>THIE6554.DIALLO</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>WESL5337.CADETTE</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>WILDINE.JEUNE</t>
-        </is>
-      </c>
-      <c r="B29" t="n">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>XUAN754N.LU</t>
-        </is>
-      </c>
-      <c r="B30" t="n">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>YATI0689.YATIN</t>
-        </is>
-      </c>
-      <c r="B31" t="n">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>ZAHIDGUL.MINHAS</t>
-        </is>
-      </c>
-      <c r="B32" t="n">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>ZAKI0190.PHILLIPHORS</t>
-        </is>
-      </c>
-      <c r="B33" t="n">
-        <v>40</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -2036,16 +1432,16 @@
         <v>20</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C2" t="n">
-        <v>-25</v>
+        <v>-11</v>
       </c>
       <c r="D2" t="n">
-        <v>-442</v>
+        <v>-366</v>
       </c>
       <c r="E2" t="n">
-        <v>-7</v>
+        <v>-257</v>
       </c>
     </row>
     <row r="3">
@@ -2053,16 +1449,16 @@
         <v>21</v>
       </c>
       <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-160</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-20</v>
+      </c>
+      <c r="E3" t="n">
         <v>-5</v>
-      </c>
-      <c r="C3" t="n">
-        <v>-264</v>
-      </c>
-      <c r="D3" t="n">
-        <v>-349</v>
-      </c>
-      <c r="E3" t="n">
-        <v>-95</v>
       </c>
     </row>
     <row r="4">
@@ -2070,16 +1466,16 @@
         <v>22</v>
       </c>
       <c r="B4" t="n">
-        <v>-9</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>-353</v>
+        <v>-162</v>
       </c>
       <c r="D4" t="n">
-        <v>-229</v>
+        <v>-96</v>
       </c>
       <c r="E4" t="n">
-        <v>-320</v>
+        <v>-84</v>
       </c>
     </row>
     <row r="5">
@@ -2087,16 +1483,16 @@
         <v>23</v>
       </c>
       <c r="B5" t="n">
-        <v>-17</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>-313</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>-34</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>-334</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -2106,16 +1502,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-31</v>
+        <v>-1</v>
       </c>
       <c r="C6" t="n">
-        <v>-955</v>
+        <v>-333</v>
       </c>
       <c r="D6" t="n">
-        <v>-1054</v>
+        <v>-482</v>
       </c>
       <c r="E6" t="n">
-        <v>-756</v>
+        <v>-346</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed replenshment to contain all bygroup
</commit_message>
<xml_diff>
--- a/pick_counts.xlsx
+++ b/pick_counts.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,14 +466,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BOHD0676.KUSHLIAK</t>
+          <t>ADOL798N.SEEMANNVAZQ</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C2" t="n">
-        <v>11.70731707317073</v>
+        <v>11.52</v>
       </c>
     </row>
     <row r="3">
@@ -483,75 +483,23 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>77</v>
+        <v>37</v>
       </c>
       <c r="C3" t="n">
-        <v>28.17073170731707</v>
+        <v>17.76</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>PATI2298.ATSIANGBE</t>
+          <t>ZAKI0190.PHILLIPHORS</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="C4" t="n">
-        <v>5.121951219512195</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>RAMI9087.SAIHI</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>46</v>
-      </c>
-      <c r="C5" t="n">
-        <v>16.82926829268293</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>TANI2739.HOSSAINISLA</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>59</v>
-      </c>
-      <c r="C6" t="n">
-        <v>21.58536585365854</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>THIE6554.DIALLO</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>46</v>
-      </c>
-      <c r="C7" t="n">
-        <v>16.82926829268293</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>XUAN754N.LU</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>72</v>
-      </c>
-      <c r="C8" t="n">
-        <v>26.34146341463414</v>
+        <v>0.96</v>
       </c>
     </row>
   </sheetData>
@@ -565,7 +513,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -593,14 +541,53 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>TANI2739.HOSSAINISLA</t>
+          <t>ASHA1141.PAGE</t>
         </is>
       </c>
       <c r="B2" t="n">
+        <v>16</v>
+      </c>
+      <c r="C2" t="n">
+        <v>7.68</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>DIAN4065.ENTRIALGO</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>15</v>
+      </c>
+      <c r="C3" t="n">
+        <v>7.199999999999999</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>KHINEHAYMAR.THAUNG</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>1</v>
       </c>
-      <c r="C2" t="n">
-        <v>0.3658536585365854</v>
+      <c r="C4" t="n">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ZAKI0190.PHILLIPHORS</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.48</v>
       </c>
     </row>
   </sheetData>
@@ -614,7 +601,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -642,118 +629,79 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BOHD0676.KUSHLIAK</t>
+          <t>BUDD0680.TENNAKOON</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="C2" t="n">
-        <v>19.02439024390244</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>JEEW9554.SITUMUDALIG</t>
+          <t>LOANA.MBONGO</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>5</v>
+        <v>128</v>
       </c>
       <c r="C3" t="n">
-        <v>1.829268292682927</v>
+        <v>61.44</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>OMAR6689.KHAN</t>
+          <t>MICA0432.RIZKALLAMAR</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
-        <v>8.780487804878049</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>RAMI9087.SAIHI</t>
+          <t>STAN9294.BAUER</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="C5" t="n">
-        <v>8.414634146341463</v>
+        <v>3.36</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>TANI2739.HOSSAINISLA</t>
+          <t>WESL5337.CADETTE</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="C6" t="n">
-        <v>6.219512195121951</v>
+        <v>24.48</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>THIE6554.DIALLO</t>
+          <t>WILDINE.JEUNE</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>72</v>
+        <v>13</v>
       </c>
       <c r="C7" t="n">
-        <v>26.34146341463414</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>WESL5337.CADETTE</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>13</v>
-      </c>
-      <c r="C8" t="n">
-        <v>4.75609756097561</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>XUAN754N.LU</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>46</v>
-      </c>
-      <c r="C9" t="n">
-        <v>16.82926829268293</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>ZAHIDGUL.MINHAS</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>81</v>
-      </c>
-      <c r="C10" t="n">
-        <v>29.63414634146341</v>
+        <v>6.239999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -795,235 +743,235 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BOHD0676.KUSHLIAK</t>
+          <t>ADOL798N.SEEMANNVAZQ</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="C2" t="n">
-        <v>3.292682926829268</v>
+        <v>15.84</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BUDD0680.TENNAKOON</t>
+          <t>ANJALI.BAKSHI</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="C3" t="n">
-        <v>4.024390243902439</v>
+        <v>1.44</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>IREN797N.CABRERA</t>
+          <t>BOHD0676.KUSHLIAK</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="C4" t="n">
-        <v>21.58536585365854</v>
+        <v>2.88</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>JEEW9554.SITUMUDALIG</t>
+          <t>BUDD0680.TENNAKOON</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C5" t="n">
-        <v>11.34146341463415</v>
+        <v>13.92</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>KADE3054.ZONGO</t>
+          <t>DIAN4065.ENTRIALGO</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="C6" t="n">
-        <v>9.146341463414634</v>
+        <v>25.92</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>LOANA.MBONGO</t>
+          <t>IREN797N.CABRERA</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="C7" t="n">
-        <v>20.48780487804878</v>
+        <v>39.84</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>LOWRHY-OTIENO.JAOKO</t>
+          <t>JEEW9554.SITUMUDALIG</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="C8" t="n">
-        <v>8.048780487804878</v>
+        <v>23.04</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MICA0432.RIZKALLAMAR</t>
+          <t>LOWRHY-OTIENO.JAOKO</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>54</v>
+        <v>107</v>
       </c>
       <c r="C9" t="n">
-        <v>19.75609756097561</v>
+        <v>51.36</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>OMAR6689.KHAN</t>
+          <t>MAKEDA.OLLIVIERRE</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>35</v>
+        <v>96</v>
       </c>
       <c r="C10" t="n">
-        <v>12.80487804878049</v>
+        <v>46.08</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>RAMI9087.SAIHI</t>
+          <t>PATI2298.ATSIANGBE</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="C11" t="n">
-        <v>6.219512195121951</v>
+        <v>17.28</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>RARG046N.YEBOAH</t>
+          <t>PATR5027.AMEH</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="C12" t="n">
-        <v>7.317073170731708</v>
+        <v>20.64</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>STAN9294.BAUER</t>
+          <t>RAMI9087.SAIHI</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C13" t="n">
-        <v>2.560975609756098</v>
+        <v>1.44</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>THIE6554.DIALLO</t>
+          <t>RARG046N.YEBOAH</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="C14" t="n">
-        <v>4.390243902439025</v>
+        <v>35.04</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>WESL5337.CADETTE</t>
+          <t>STAN9294.BAUER</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="C15" t="n">
-        <v>10.97560975609756</v>
+        <v>26.4</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>WILDINE.JEUNE</t>
+          <t>THIE6554.DIALLO</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="C16" t="n">
-        <v>9.512195121951219</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>XUAN754N.LU</t>
+          <t>WESL5337.CADETTE</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="C17" t="n">
-        <v>1.463414634146341</v>
+        <v>30.24</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>ZAHIDGUL.MINHAS</t>
+          <t>WILDINE.JEUNE</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>32</v>
+        <v>95</v>
       </c>
       <c r="C18" t="n">
-        <v>11.70731707317073</v>
+        <v>45.59999999999999</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>ZAKI0190.PHILLIPHORS</t>
+          <t>ZAHIDGUL.MINHAS</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="C19" t="n">
-        <v>11.70731707317073</v>
+        <v>1.44</v>
       </c>
     </row>
   </sheetData>
@@ -1037,7 +985,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1065,79 +1013,118 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BOHD0676.KUSHLIAK</t>
+          <t>ADOL798N.SEEMANNVAZQ</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="C2" t="n">
-        <v>32.5609756097561</v>
+        <v>54.23999999999999</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>OMAR6689.KHAN</t>
+          <t>DIAN4065.ENTRIALGO</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10</v>
+        <v>76</v>
       </c>
       <c r="C3" t="n">
-        <v>3.658536585365854</v>
+        <v>36.48</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>RAMI9087.SAIHI</t>
+          <t>ESSE0616.UDEH</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="C4" t="n">
-        <v>14.63414634146342</v>
+        <v>41.27999999999999</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>TANI2739.HOSSAINISLA</t>
+          <t>MARI882N.ABDELKADER</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>19</v>
+        <v>124</v>
       </c>
       <c r="C5" t="n">
-        <v>6.951219512195122</v>
+        <v>59.52</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>THIE6554.DIALLO</t>
+          <t>RAMI9087.SAIHI</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>21.58536585365854</v>
+        <v>3.84</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>XUAN754N.LU</t>
+          <t>RARG046N.YEBOAH</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C7" t="n">
-        <v>1.463414634146341</v>
+        <v>7.68</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>STAN9294.BAUER</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>25</v>
+      </c>
+      <c r="C8" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>TANI2739.HOSSAINISLA</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>20</v>
+      </c>
+      <c r="C9" t="n">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>WESL5337.CADETTE</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>63</v>
+      </c>
+      <c r="C10" t="n">
+        <v>30.24</v>
       </c>
     </row>
   </sheetData>
@@ -1151,7 +1138,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1174,211 +1161,261 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BOHD0676.KUSHLIAK</t>
+          <t>ADOL798N.SEEMANNVAZQ</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>35</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BUDD0680.TENNAKOON</t>
+          <t>ANJALI.BAKSHI</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>22</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>DIAN4065.ENTRIALGO</t>
+          <t>ASHA1141.PAGE</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>150</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>IREN797N.CABRERA</t>
+          <t>BOHD0676.KUSHLIAK</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>142</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>JEEW9554.SITUMUDALIG</t>
+          <t>BUDD0680.TENNAKOON</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>138</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>KADE3054.ZONGO</t>
+          <t>DIAN4065.ENTRIALGO</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>134</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>LOANA.MBONGO</t>
+          <t>ESSE0616.UDEH</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>142</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>LOWRHY-OTIENO.JAOKO</t>
+          <t>IREN797N.CABRERA</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>136</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>MICA0432.RIZKALLAMAR</t>
+          <t>JEEW9554.SITUMUDALIG</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>144</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>OMAR6689.KHAN</t>
+          <t>KHINEHAYMAR.THAUNG</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>51</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>PATI2298.ATSIANGBE</t>
+          <t>LOANA.MBONGO</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>RAMI9087.SAIHI</t>
+          <t>LOWRHY-OTIENO.JAOKO</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>48</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>RARG046N.YEBOAH</t>
+          <t>MAKEDA.OLLIVIERRE</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>152</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>STAN9294.BAUER</t>
+          <t>MARI882N.ABDELKADER</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>170</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>TANI2739.HOSSAINISLA</t>
+          <t>MICA0432.RIZKALLAMAR</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>74</v>
+        <v>124</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>THIE6554.DIALLO</t>
+          <t>PATI2298.ATSIANGBE</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>37</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>WESL5337.CADETTE</t>
+          <t>PATR5027.AMEH</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>132</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>WILDINE.JEUNE</t>
+          <t>RAMI9087.SAIHI</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>135</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>XUAN754N.LU</t>
+          <t>RARG046N.YEBOAH</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>63</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>ZAHIDGUL.MINHAS</t>
+          <t>STAN9294.BAUER</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>59</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>TANI2739.HOSSAINISLA</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>THIE6554.DIALLO</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>WESL5337.CADETTE</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>WILDINE.JEUNE</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>ZAHIDGUL.MINHAS</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
           <t>ZAKI0190.PHILLIPHORS</t>
         </is>
       </c>
-      <c r="B22" t="n">
-        <v>135</v>
+      <c r="B27" t="n">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1432,16 +1469,16 @@
         <v>20</v>
       </c>
       <c r="B2" t="n">
-        <v>-1</v>
+        <v>-16</v>
       </c>
       <c r="C2" t="n">
-        <v>-11</v>
+        <v>-40</v>
       </c>
       <c r="D2" t="n">
-        <v>-366</v>
+        <v>-396</v>
       </c>
       <c r="E2" t="n">
-        <v>-257</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -1449,16 +1486,16 @@
         <v>21</v>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C3" t="n">
-        <v>-160</v>
+        <v>-137</v>
       </c>
       <c r="D3" t="n">
-        <v>-20</v>
+        <v>-399</v>
       </c>
       <c r="E3" t="n">
-        <v>-5</v>
+        <v>-63</v>
       </c>
     </row>
     <row r="4">
@@ -1466,16 +1503,16 @@
         <v>22</v>
       </c>
       <c r="B4" t="n">
+        <v>-16</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-32</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-40</v>
+      </c>
+      <c r="E4" t="n">
         <v>0</v>
-      </c>
-      <c r="C4" t="n">
-        <v>-162</v>
-      </c>
-      <c r="D4" t="n">
-        <v>-96</v>
-      </c>
-      <c r="E4" t="n">
-        <v>-84</v>
       </c>
     </row>
     <row r="5">
@@ -1502,16 +1539,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-1</v>
+        <v>-33</v>
       </c>
       <c r="C6" t="n">
-        <v>-333</v>
+        <v>-209</v>
       </c>
       <c r="D6" t="n">
-        <v>-482</v>
+        <v>-835</v>
       </c>
       <c r="E6" t="n">
-        <v>-346</v>
+        <v>-63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
styled the user_data html page
</commit_message>
<xml_diff>
--- a/pick_counts.xlsx
+++ b/pick_counts.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,36 +470,88 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C2" t="n">
-        <v>11.52</v>
+        <v>14.18181818181818</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DIAN4065.ENTRIALGO</t>
+          <t>BOHD0676.KUSHLIAK</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>17.76</v>
+        <v>1.090909090909091</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ZAKI0190.PHILLIPHORS</t>
+          <t>DIAN4065.ENTRIALGO</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2</v>
+        <v>67</v>
       </c>
       <c r="C4" t="n">
-        <v>0.96</v>
+        <v>36.54545454545455</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>PATR5027.AMEH</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1.636363636363636</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>THIE6554.DIALLO</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>14</v>
+      </c>
+      <c r="C6" t="n">
+        <v>7.636363636363637</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>XUAN754N.LU</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>3</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1.636363636363636</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ZAHIDGUL.MINHAS</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>4</v>
+      </c>
+      <c r="C8" t="n">
+        <v>2.181818181818182</v>
       </c>
     </row>
   </sheetData>
@@ -541,14 +593,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ASHA1141.PAGE</t>
+          <t>BOHD0676.KUSHLIAK</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="C2" t="n">
-        <v>7.68</v>
+        <v>2.181818181818182</v>
       </c>
     </row>
     <row r="3">
@@ -558,36 +610,36 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="C3" t="n">
-        <v>7.199999999999999</v>
+        <v>26.72727272727273</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>KHINEHAYMAR.THAUNG</t>
+          <t>PATR5027.AMEH</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" t="n">
-        <v>0.48</v>
+        <v>1.090909090909091</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ZAKI0190.PHILLIPHORS</t>
+          <t>ZAHIDGUL.MINHAS</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>0.48</v>
+        <v>1.636363636363636</v>
       </c>
     </row>
   </sheetData>
@@ -601,7 +653,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -629,79 +681,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BUDD0680.TENNAKOON</t>
+          <t>REJWAN.ISLAM</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C2" t="n">
-        <v>2.4</v>
+        <v>9.818181818181818</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>LOANA.MBONGO</t>
+          <t>WESL5337.CADETTE</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>128</v>
+        <v>41</v>
       </c>
       <c r="C3" t="n">
-        <v>61.44</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>MICA0432.RIZKALLAMAR</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>5</v>
-      </c>
-      <c r="C4" t="n">
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>STAN9294.BAUER</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>7</v>
-      </c>
-      <c r="C5" t="n">
-        <v>3.36</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>WESL5337.CADETTE</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>51</v>
-      </c>
-      <c r="C6" t="n">
-        <v>24.48</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>WILDINE.JEUNE</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>13</v>
-      </c>
-      <c r="C7" t="n">
-        <v>6.239999999999999</v>
+        <v>22.36363636363636</v>
       </c>
     </row>
   </sheetData>
@@ -715,7 +715,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -743,40 +743,40 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ADOL798N.SEEMANNVAZQ</t>
+          <t>AHME0710.JUBRAN</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="C2" t="n">
-        <v>15.84</v>
+        <v>5.454545454545455</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ANJALI.BAKSHI</t>
+          <t>ANASTASIIA.MAKHTOUT</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3</v>
+        <v>93</v>
       </c>
       <c r="C3" t="n">
-        <v>1.44</v>
+        <v>50.72727272727273</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>BOHD0676.KUSHLIAK</t>
+          <t>ANJALI.BAKSHI</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6</v>
+        <v>94</v>
       </c>
       <c r="C4" t="n">
-        <v>2.88</v>
+        <v>51.27272727272727</v>
       </c>
     </row>
     <row r="5">
@@ -786,192 +786,231 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="C5" t="n">
-        <v>13.92</v>
+        <v>43.09090909090909</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DIAN4065.ENTRIALGO</t>
+          <t>DEVI789.SINGH</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="C6" t="n">
-        <v>25.92</v>
+        <v>19.09090909090909</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>IREN797N.CABRERA</t>
+          <t>GIGNESH.PATEL</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>83</v>
+        <v>34</v>
       </c>
       <c r="C7" t="n">
-        <v>39.84</v>
+        <v>18.54545454545455</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>JEEW9554.SITUMUDALIG</t>
+          <t>IREN797N.CABRERA</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="C8" t="n">
-        <v>23.04</v>
+        <v>35.45454545454545</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>LOWRHY-OTIENO.JAOKO</t>
+          <t>JEEW9554.SITUMUDALIG</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>107</v>
+        <v>132</v>
       </c>
       <c r="C9" t="n">
-        <v>51.36</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>MAKEDA.OLLIVIERRE</t>
+          <t>KADE3054.ZONGO</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>96</v>
+        <v>51</v>
       </c>
       <c r="C10" t="n">
-        <v>46.08</v>
+        <v>27.81818181818182</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>PATI2298.ATSIANGBE</t>
+          <t>LOWRHY-OTIENO.JAOKO</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>36</v>
+        <v>99</v>
       </c>
       <c r="C11" t="n">
-        <v>17.28</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>PATR5027.AMEH</t>
+          <t>MICA0432.RIZKALLAMAR</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>43</v>
+        <v>111</v>
       </c>
       <c r="C12" t="n">
-        <v>20.64</v>
+        <v>60.54545454545455</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>RAMI9087.SAIHI</t>
+          <t>PATI2298.ATSIANGBE</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="C13" t="n">
-        <v>1.44</v>
+        <v>13.09090909090909</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>RARG046N.YEBOAH</t>
+          <t>PRINCE.FORSON</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="C14" t="n">
-        <v>35.04</v>
+        <v>26.18181818181818</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>STAN9294.BAUER</t>
+          <t>REJWAN.ISLAM</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C15" t="n">
-        <v>26.4</v>
+        <v>21.81818181818182</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>THIE6554.DIALLO</t>
+          <t>STAN9294.BAUER</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="C16" t="n">
-        <v>2.4</v>
+        <v>33.27272727272727</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>WESL5337.CADETTE</t>
+          <t>SURESH.DHAWAN</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="C17" t="n">
-        <v>30.24</v>
+        <v>19.63636363636364</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>WILDINE.JEUNE</t>
+          <t>THIE6554.DIALLO</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="C18" t="n">
-        <v>45.59999999999999</v>
+        <v>38.18181818181818</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>ZAHIDGUL.MINHAS</t>
+          <t>WESL5337.CADETTE</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>3</v>
+        <v>62</v>
       </c>
       <c r="C19" t="n">
-        <v>1.44</v>
+        <v>33.81818181818182</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>XUAN754N.LU</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>59</v>
+      </c>
+      <c r="C20" t="n">
+        <v>32.18181818181818</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>YATI0689.YATIN</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>38</v>
+      </c>
+      <c r="C21" t="n">
+        <v>20.72727272727273</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>ZAKI0190.PHILLIPHORS</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>115</v>
+      </c>
+      <c r="C22" t="n">
+        <v>62.72727272727273</v>
       </c>
     </row>
   </sheetData>
@@ -985,7 +1024,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1017,114 +1056,179 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C2" t="n">
-        <v>54.23999999999999</v>
+        <v>62.72727272727273</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DIAN4065.ENTRIALGO</t>
+          <t>BOHD0676.KUSHLIAK</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>76</v>
+        <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>36.48</v>
+        <v>1.090909090909091</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ESSE0616.UDEH</t>
+          <t>DEVI789.SINGH</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>86</v>
+        <v>27</v>
       </c>
       <c r="C4" t="n">
-        <v>41.27999999999999</v>
+        <v>14.72727272727273</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>MARI882N.ABDELKADER</t>
+          <t>DIAN4065.ENTRIALGO</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>124</v>
+        <v>59</v>
       </c>
       <c r="C5" t="n">
-        <v>59.52</v>
+        <v>32.18181818181818</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>RAMI9087.SAIHI</t>
+          <t>ESSE0616.UDEH</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="C6" t="n">
-        <v>3.84</v>
+        <v>35.45454545454545</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>RARG046N.YEBOAH</t>
+          <t>KADE3054.ZONGO</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C7" t="n">
-        <v>7.68</v>
+        <v>15.27272727272727</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>STAN9294.BAUER</t>
+          <t>MICA0432.RIZKALLAMAR</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>25</v>
+        <v>111</v>
       </c>
       <c r="C8" t="n">
-        <v>12</v>
+        <v>60.54545454545455</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>TANI2739.HOSSAINISLA</t>
+          <t>NESR2403.ATTALAH</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C9" t="n">
-        <v>9.6</v>
+        <v>16.90909090909091</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>STAN9294.BAUER</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>60</v>
+      </c>
+      <c r="C10" t="n">
+        <v>32.72727272727273</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>SURESH.DHAWAN</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>123</v>
+      </c>
+      <c r="C11" t="n">
+        <v>67.09090909090909</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>THIE6554.DIALLO</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>159</v>
+      </c>
+      <c r="C12" t="n">
+        <v>86.72727272727273</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
           <t>WESL5337.CADETTE</t>
         </is>
       </c>
-      <c r="B10" t="n">
-        <v>63</v>
-      </c>
-      <c r="C10" t="n">
-        <v>30.24</v>
+      <c r="B13" t="n">
+        <v>61</v>
+      </c>
+      <c r="C13" t="n">
+        <v>33.27272727272727</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>XUAN754N.LU</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>59</v>
+      </c>
+      <c r="C14" t="n">
+        <v>32.18181818181818</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>YATI0689.YATIN</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>97</v>
+      </c>
+      <c r="C15" t="n">
+        <v>52.90909090909091</v>
       </c>
     </row>
   </sheetData>
@@ -1138,7 +1242,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1165,113 +1269,113 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>52</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ANJALI.BAKSHI</t>
+          <t>AHME0710.JUBRAN</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>124</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ASHA1141.PAGE</t>
+          <t>ANASTASIIA.MAKHTOUT</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>BOHD0676.KUSHLIAK</t>
+          <t>ANJALI.BAKSHI</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>119</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>BUDD0680.TENNAKOON</t>
+          <t>BOHD0676.KUSHLIAK</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>DIAN4065.ENTRIALGO</t>
+          <t>BUDD0680.TENNAKOON</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>39</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ESSE0616.UDEH</t>
+          <t>DEVI789.SINGH</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>97</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>IREN797N.CABRERA</t>
+          <t>DIAN4065.ENTRIALGO</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>JEEW9554.SITUMUDALIG</t>
+          <t>ESSE0616.UDEH</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>22</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>KHINEHAYMAR.THAUNG</t>
+          <t>GIGNESH.PATEL</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>88</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>LOANA.MBONGO</t>
+          <t>IREN797N.CABRERA</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>33</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>LOWRHY-OTIENO.JAOKO</t>
+          <t>JEEW9554.SITUMUDALIG</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -1281,141 +1385,131 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>MAKEDA.OLLIVIERRE</t>
+          <t>LOWRHY-OTIENO.JAOKO</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>MARI882N.ABDELKADER</t>
+          <t>NESR2403.ATTALAH</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>85</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>MICA0432.RIZKALLAMAR</t>
+          <t>PATI2298.ATSIANGBE</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>124</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>PATI2298.ATSIANGBE</t>
+          <t>PATR5027.AMEH</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>PATR5027.AMEH</t>
+          <t>PRINCE.FORSON</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>49</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>RAMI9087.SAIHI</t>
+          <t>REJWAN.ISLAM</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>117</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>RARG046N.YEBOAH</t>
+          <t>SURESH.DHAWAN</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>41</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>STAN9294.BAUER</t>
+          <t>THIE6554.DIALLO</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>TANI2739.HOSSAINISLA</t>
+          <t>WESL5337.CADETTE</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>116</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>THIE6554.DIALLO</t>
+          <t>XUAN754N.LU</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>120</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>WESL5337.CADETTE</t>
+          <t>YATI0689.YATIN</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>28</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>WILDINE.JEUNE</t>
+          <t>ZAHIDGUL.MINHAS</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>36</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>ZAHIDGUL.MINHAS</t>
+          <t>ZAKI0190.PHILLIPHORS</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>ZAKI0190.PHILLIPHORS</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>112</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1469,16 +1563,16 @@
         <v>20</v>
       </c>
       <c r="B2" t="n">
-        <v>-16</v>
+        <v>-26</v>
       </c>
       <c r="C2" t="n">
-        <v>-40</v>
+        <v>-32</v>
       </c>
       <c r="D2" t="n">
-        <v>-396</v>
+        <v>-594</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="3">
@@ -1486,16 +1580,16 @@
         <v>21</v>
       </c>
       <c r="B3" t="n">
-        <v>-1</v>
+        <v>-32</v>
       </c>
       <c r="C3" t="n">
-        <v>-137</v>
+        <v>-24</v>
       </c>
       <c r="D3" t="n">
-        <v>-399</v>
+        <v>-751</v>
       </c>
       <c r="E3" t="n">
-        <v>-63</v>
+        <v>-106</v>
       </c>
     </row>
     <row r="4">
@@ -1503,16 +1597,16 @@
         <v>22</v>
       </c>
       <c r="B4" t="n">
-        <v>-16</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>-32</v>
+        <v>-3</v>
       </c>
       <c r="D4" t="n">
-        <v>-40</v>
+        <v>-11</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>-12</v>
       </c>
     </row>
     <row r="5">
@@ -1539,16 +1633,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-33</v>
+        <v>-58</v>
       </c>
       <c r="C6" t="n">
-        <v>-209</v>
+        <v>-59</v>
       </c>
       <c r="D6" t="n">
-        <v>-835</v>
+        <v>-1356</v>
       </c>
       <c r="E6" t="n">
-        <v>-63</v>
+        <v>-119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>